<commit_message>
Fixed: 1) Not able to read in date 2) Infinite view in ProjectListingView
</commit_message>
<xml_diff>
--- a/data/project/ProjectDetails.xlsx
+++ b/data/project/ProjectDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grey Bunny\Desktop\FCS5-Grp5\data\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AEA457-DB8A-43CA-A91B-4493C16DB2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5483B27D-35BD-4F3B-A43B-5771D5A84169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2385" yWindow="1860" windowWidth="24660" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>projectId</t>
   </si>
@@ -47,12 +47,6 @@
   </si>
   <si>
     <t>closingDate</t>
-  </si>
-  <si>
-    <t>2/15/2025</t>
-  </si>
-  <si>
-    <t>3/20/2025</t>
   </si>
 </sst>
 </file>
@@ -86,8 +80,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,7 +390,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,11 +436,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
+      <c r="D2" s="1">
+        <v>45703</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45736</v>
       </c>
       <c r="F2">
         <v>3</v>

</xml_diff>

<commit_message>
1) Generated various test cases in xlsx files
</commit_message>
<xml_diff>
--- a/data/project/ProjectDetails.xlsx
+++ b/data/project/ProjectDetails.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grey Bunny\Desktop\FCS5-Grp5\data\project\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>projectId</t>
   </si>
@@ -47,12 +47,27 @@
   </si>
   <si>
     <t>closingDate</t>
+  </si>
+  <si>
+    <t>TestProjectOne</t>
+  </si>
+  <si>
+    <t>Yishun</t>
+  </si>
+  <si>
+    <t>TestProject2</t>
+  </si>
+  <si>
+    <t>YishunAgain</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/MM/yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,9 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -395,58 +412,104 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.28515625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.42578125"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="11.28515625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>45703.0</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>45736.0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G2" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>45741.0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>45773.0</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="G3" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>45713.0</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>45940.0</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="G4" t="b" s="0">
         <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1">
-        <v>45703</v>
-      </c>
-      <c r="E2" s="1">
-        <v>45736</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "1) Added Javadoc"
This reverts commit e8720a33eaf8dff808aaa7c98938384bb1216ba7.
</commit_message>
<xml_diff>
--- a/data/project/ProjectDetails.xlsx
+++ b/data/project/ProjectDetails.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>projectId</t>
   </si>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t>YishunAgain</t>
-  </si>
-  <si>
-    <t>TestProject</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -101,10 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
@@ -411,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -519,29 +512,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>45772.0</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>45773.0</v>
-      </c>
-      <c r="F5" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="G5" t="b" s="0">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/IAmGreyBunny/FCS5-Grp5"
This reverts commit be1511047ae465f731e303b9131dc7c1d5ecd3a9, reversing
changes made to 924224b65724dcf87d0b51c107c6f7ad9dee85c1.
</commit_message>
<xml_diff>
--- a/data/project/ProjectDetails.xlsx
+++ b/data/project/ProjectDetails.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>projectId</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>YishunAgain</t>
+  </si>
+  <si>
+    <t>TestProject</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -95,9 +101,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
@@ -404,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -512,6 +519,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>45772.0</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>45773.0</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="G5" t="b" s="0">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reapply "Merge branch 'main' of https://github.com/IAmGreyBunny/FCS5-Grp5"
This reverts commit d9225ac389852bc7bd610aa649cb3c985f8e4043.
</commit_message>
<xml_diff>
--- a/data/project/ProjectDetails.xlsx
+++ b/data/project/ProjectDetails.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>projectId</t>
   </si>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t>YishunAgain</t>
-  </si>
-  <si>
-    <t>TestProject</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -101,10 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
@@ -411,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -519,29 +512,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>45772.0</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>45773.0</v>
-      </c>
-      <c r="F5" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="G5" t="b" s="0">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>